<commit_message>
data till 27Jan 8:30AM
</commit_message>
<xml_diff>
--- a/Daily Orders/January-2021-RetailerWiseOrder.xlsx
+++ b/Daily Orders/January-2021-RetailerWiseOrder.xlsx
@@ -682,11 +682,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
+    <numFmt numFmtId="176" formatCode="[$-409]d\-mmm;@"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="[$-409]d\-mmm;@"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -706,36 +706,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -750,7 +720,38 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -764,9 +765,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -781,23 +782,8 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -811,6 +797,15 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -825,14 +820,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
@@ -841,7 +828,20 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -911,7 +911,133 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -923,133 +1049,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1061,13 +1061,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1085,13 +1085,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1102,6 +1102,30 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -1122,39 +1146,6 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -1167,8 +1158,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1202,18 +1193,27 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1225,134 +1225,134 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="20" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="23" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="26" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="23" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="24" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="24" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1385,9 +1385,6 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
@@ -1769,11 +1766,11 @@
   <dimension ref="A1:AS108"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="7" ySplit="2" topLeftCell="AF28" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="7" ySplit="2" topLeftCell="AF47" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="B31" sqref="B31"/>
+      <selection pane="bottomRight" activeCell="AG50" sqref="AG50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -1813,129 +1810,129 @@
       <c r="H1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="19">
+      <c r="I1" s="18">
         <v>43831</v>
       </c>
-      <c r="J1" s="19">
+      <c r="J1" s="18">
         <v>43832</v>
       </c>
-      <c r="K1" s="19">
+      <c r="K1" s="18">
         <v>43833</v>
       </c>
-      <c r="L1" s="19">
+      <c r="L1" s="18">
         <v>43834</v>
       </c>
-      <c r="M1" s="19">
+      <c r="M1" s="18">
         <v>43835</v>
       </c>
-      <c r="N1" s="19">
+      <c r="N1" s="18">
         <v>43836</v>
       </c>
-      <c r="O1" s="19">
+      <c r="O1" s="18">
         <v>43837</v>
       </c>
-      <c r="P1" s="19">
+      <c r="P1" s="18">
         <v>43838</v>
       </c>
-      <c r="Q1" s="19">
+      <c r="Q1" s="18">
         <v>43839</v>
       </c>
-      <c r="R1" s="19">
+      <c r="R1" s="18">
         <v>43840</v>
       </c>
-      <c r="S1" s="19">
+      <c r="S1" s="18">
         <v>43841</v>
       </c>
-      <c r="T1" s="19">
+      <c r="T1" s="18">
         <v>43842</v>
       </c>
-      <c r="U1" s="19">
+      <c r="U1" s="18">
         <v>43843</v>
       </c>
-      <c r="V1" s="19">
+      <c r="V1" s="18">
         <v>43844</v>
       </c>
-      <c r="W1" s="19">
+      <c r="W1" s="18">
         <v>43845</v>
       </c>
-      <c r="X1" s="19">
+      <c r="X1" s="18">
         <v>43846</v>
       </c>
-      <c r="Y1" s="19">
+      <c r="Y1" s="18">
         <v>43847</v>
       </c>
-      <c r="Z1" s="19">
+      <c r="Z1" s="18">
         <v>43848</v>
       </c>
-      <c r="AA1" s="19">
+      <c r="AA1" s="18">
         <v>43849</v>
       </c>
-      <c r="AB1" s="19">
+      <c r="AB1" s="18">
         <v>43850</v>
       </c>
-      <c r="AC1" s="19">
+      <c r="AC1" s="18">
         <v>43851</v>
       </c>
-      <c r="AD1" s="19">
+      <c r="AD1" s="18">
         <v>43852</v>
       </c>
-      <c r="AE1" s="19">
+      <c r="AE1" s="18">
         <v>43853</v>
       </c>
-      <c r="AF1" s="19">
+      <c r="AF1" s="18">
         <v>43854</v>
       </c>
-      <c r="AG1" s="19">
+      <c r="AG1" s="18">
         <v>43855</v>
       </c>
-      <c r="AH1" s="19">
+      <c r="AH1" s="18">
         <v>43856</v>
       </c>
-      <c r="AI1" s="19">
+      <c r="AI1" s="18">
         <v>43857</v>
       </c>
-      <c r="AJ1" s="19">
+      <c r="AJ1" s="18">
         <v>43858</v>
       </c>
-      <c r="AK1" s="19">
+      <c r="AK1" s="18">
         <v>43859</v>
       </c>
-      <c r="AL1" s="19">
+      <c r="AL1" s="18">
         <v>43860</v>
       </c>
-      <c r="AM1" s="19">
+      <c r="AM1" s="18">
         <v>43861</v>
       </c>
-      <c r="AN1" s="21"/>
-      <c r="AO1" s="21"/>
-      <c r="AP1" s="21"/>
-      <c r="AQ1" s="21"/>
-      <c r="AR1" s="21"/>
-      <c r="AS1" s="21"/>
+      <c r="AN1" s="20"/>
+      <c r="AO1" s="20"/>
+      <c r="AP1" s="20"/>
+      <c r="AQ1" s="20"/>
+      <c r="AR1" s="20"/>
+      <c r="AS1" s="20"/>
     </row>
     <row r="2" s="2" customFormat="1" spans="1:39">
       <c r="A2" s="8"/>
       <c r="B2" s="9">
         <f>SUM(F3:F120)</f>
-        <v>1306500</v>
-      </c>
-      <c r="C2" s="10"/>
-      <c r="D2" s="11">
+        <v>1326500</v>
+      </c>
+      <c r="C2" s="1"/>
+      <c r="D2" s="10">
         <f>SUM(G3:G120)</f>
-        <v>1235000</v>
-      </c>
-      <c r="E2" s="12" t="s">
+        <v>1255800</v>
+      </c>
+      <c r="E2" s="11" t="s">
         <v>8</v>
       </c>
       <c r="F2" s="9">
         <f>G2/1.04+H2</f>
-        <v>1306500</v>
-      </c>
-      <c r="G2" s="11">
+        <v>1326500</v>
+      </c>
+      <c r="G2" s="10">
         <f t="shared" ref="G2:G16" si="0">SUM(I2:AM2)</f>
-        <v>1235000</v>
-      </c>
-      <c r="H2" s="13">
+        <v>1255800</v>
+      </c>
+      <c r="H2" s="12">
         <f>SUM(H3:H120)</f>
         <v>119000</v>
       </c>
@@ -2045,7 +2042,7 @@
       </c>
       <c r="AI2" s="2">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>20800</v>
       </c>
       <c r="AJ2" s="2">
         <f t="shared" si="1"/>
@@ -2071,7 +2068,7 @@
       <c r="D3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="14" t="s">
+      <c r="E3" s="13" t="s">
         <v>10</v>
       </c>
       <c r="F3" s="1">
@@ -2082,7 +2079,7 @@
         <f t="shared" si="0"/>
         <v>9360</v>
       </c>
-      <c r="H3" s="15">
+      <c r="H3" s="14">
         <v>3000</v>
       </c>
       <c r="I3" s="4"/>
@@ -2103,7 +2100,7 @@
       <c r="V3" s="4"/>
       <c r="W3" s="4"/>
       <c r="X3" s="4"/>
-      <c r="Y3" s="20">
+      <c r="Y3" s="19">
         <v>3120</v>
       </c>
       <c r="Z3" s="4"/>
@@ -2130,7 +2127,7 @@
       <c r="D4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="14" t="s">
+      <c r="E4" s="13" t="s">
         <v>11</v>
       </c>
       <c r="F4" s="1">
@@ -2141,7 +2138,7 @@
         <f t="shared" si="0"/>
         <v>4680</v>
       </c>
-      <c r="H4" s="15">
+      <c r="H4" s="14">
         <v>0</v>
       </c>
       <c r="I4" s="4"/>
@@ -2154,7 +2151,7 @@
       <c r="P4" s="4"/>
       <c r="Q4" s="4"/>
       <c r="R4" s="4"/>
-      <c r="S4" s="20">
+      <c r="S4" s="19">
         <v>1560</v>
       </c>
       <c r="T4" s="4"/>
@@ -2192,18 +2189,18 @@
       <c r="D5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="14" t="s">
+      <c r="E5" s="13" t="s">
         <v>13</v>
       </c>
       <c r="F5" s="1">
         <f t="shared" si="2"/>
-        <v>12000</v>
+        <v>13000</v>
       </c>
       <c r="G5" s="1">
         <f t="shared" si="0"/>
-        <v>12480</v>
-      </c>
-      <c r="H5" s="15">
+        <v>13520</v>
+      </c>
+      <c r="H5" s="14">
         <v>0</v>
       </c>
       <c r="I5" s="4">
@@ -2254,7 +2251,9 @@
       <c r="AH5" s="4">
         <v>1040</v>
       </c>
-      <c r="AI5" s="4"/>
+      <c r="AI5" s="4">
+        <v>1040</v>
+      </c>
       <c r="AJ5" s="4"/>
       <c r="AK5" s="4"/>
       <c r="AL5" s="4"/>
@@ -2270,7 +2269,7 @@
       <c r="D6" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E6" s="14" t="s">
+      <c r="E6" s="13" t="s">
         <v>15</v>
       </c>
       <c r="F6" s="1">
@@ -2281,7 +2280,7 @@
         <f t="shared" si="0"/>
         <v>20800</v>
       </c>
-      <c r="H6" s="15">
+      <c r="H6" s="14">
         <v>3000</v>
       </c>
       <c r="I6" s="4"/>
@@ -2334,7 +2333,7 @@
       <c r="D7" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="14" t="s">
+      <c r="E7" s="13" t="s">
         <v>17</v>
       </c>
       <c r="F7" s="1">
@@ -2345,7 +2344,7 @@
         <f t="shared" si="0"/>
         <v>57200</v>
       </c>
-      <c r="H7" s="15">
+      <c r="H7" s="14">
         <v>10000</v>
       </c>
       <c r="I7" s="4">
@@ -2434,7 +2433,7 @@
       <c r="D8" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E8" s="14" t="s">
+      <c r="E8" s="13" t="s">
         <v>19</v>
       </c>
       <c r="F8" s="1">
@@ -2445,7 +2444,7 @@
         <f t="shared" si="0"/>
         <v>6240</v>
       </c>
-      <c r="H8" s="15">
+      <c r="H8" s="14">
         <v>0</v>
       </c>
       <c r="I8" s="4"/>
@@ -2493,7 +2492,7 @@
       <c r="D9" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E9" s="14" t="s">
+      <c r="E9" s="13" t="s">
         <v>20</v>
       </c>
       <c r="F9" s="1">
@@ -2504,7 +2503,7 @@
         <f t="shared" si="0"/>
         <v>6240</v>
       </c>
-      <c r="H9" s="15">
+      <c r="H9" s="14">
         <v>0</v>
       </c>
       <c r="I9" s="4"/>
@@ -2555,7 +2554,7 @@
       <c r="D10" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E10" s="14" t="s">
+      <c r="E10" s="13" t="s">
         <v>22</v>
       </c>
       <c r="F10" s="1">
@@ -2566,7 +2565,7 @@
         <f t="shared" si="0"/>
         <v>31200</v>
       </c>
-      <c r="H10" s="15">
+      <c r="H10" s="14">
         <v>0</v>
       </c>
       <c r="I10" s="4"/>
@@ -2620,7 +2619,7 @@
       <c r="D11" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E11" s="14" t="s">
+      <c r="E11" s="13" t="s">
         <v>24</v>
       </c>
       <c r="F11" s="1">
@@ -2631,7 +2630,7 @@
         <f t="shared" si="0"/>
         <v>14560</v>
       </c>
-      <c r="H11" s="15">
+      <c r="H11" s="14">
         <v>2000</v>
       </c>
       <c r="I11" s="4"/>
@@ -2687,7 +2686,7 @@
       <c r="D12" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E12" s="14" t="s">
+      <c r="E12" s="13" t="s">
         <v>25</v>
       </c>
       <c r="F12" s="1">
@@ -2698,7 +2697,7 @@
         <f t="shared" si="0"/>
         <v>7280</v>
       </c>
-      <c r="H12" s="15">
+      <c r="H12" s="14">
         <v>0</v>
       </c>
       <c r="I12" s="4"/>
@@ -2753,7 +2752,7 @@
       <c r="D13" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E13" s="14" t="s">
+      <c r="E13" s="13" t="s">
         <v>26</v>
       </c>
       <c r="F13" s="1">
@@ -2764,7 +2763,7 @@
         <f t="shared" si="0"/>
         <v>31200</v>
       </c>
-      <c r="H13" s="15">
+      <c r="H13" s="14">
         <v>0</v>
       </c>
       <c r="I13" s="4"/>
@@ -2818,7 +2817,7 @@
       <c r="D14" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E14" s="14" t="s">
+      <c r="E14" s="13" t="s">
         <v>27</v>
       </c>
       <c r="F14" s="1">
@@ -2829,7 +2828,7 @@
         <f t="shared" si="0"/>
         <v>52000</v>
       </c>
-      <c r="H14" s="15">
+      <c r="H14" s="14">
         <v>5000</v>
       </c>
       <c r="I14" s="4"/>
@@ -2894,7 +2893,7 @@
       <c r="D15" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E15" s="14" t="s">
+      <c r="E15" s="13" t="s">
         <v>29</v>
       </c>
       <c r="F15" s="1">
@@ -2905,7 +2904,7 @@
         <f t="shared" si="0"/>
         <v>10400</v>
       </c>
-      <c r="H15" s="15">
+      <c r="H15" s="14">
         <v>0</v>
       </c>
       <c r="I15" s="4"/>
@@ -2957,7 +2956,7 @@
       <c r="D16" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E16" s="14" t="s">
+      <c r="E16" s="13" t="s">
         <v>30</v>
       </c>
       <c r="F16" s="1">
@@ -2968,12 +2967,12 @@
         <f t="shared" si="0"/>
         <v>3120</v>
       </c>
-      <c r="H16" s="15">
+      <c r="H16" s="14">
         <v>500</v>
       </c>
       <c r="I16" s="4"/>
       <c r="J16" s="4"/>
-      <c r="K16" s="20">
+      <c r="K16" s="19">
         <v>1040</v>
       </c>
       <c r="L16" s="4"/>
@@ -3016,7 +3015,7 @@
       <c r="D17" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E17" s="14" t="s">
+      <c r="E17" s="13" t="s">
         <v>31</v>
       </c>
       <c r="F17" s="1">
@@ -3027,7 +3026,7 @@
         <f t="shared" ref="G17:G35" si="3">SUM(I17:AM17)</f>
         <v>21840</v>
       </c>
-      <c r="H17" s="15">
+      <c r="H17" s="14">
         <v>0</v>
       </c>
       <c r="I17" s="4">
@@ -3083,7 +3082,7 @@
       <c r="D18" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="E18" s="14" t="s">
+      <c r="E18" s="13" t="s">
         <v>33</v>
       </c>
       <c r="F18" s="1">
@@ -3094,7 +3093,7 @@
         <f t="shared" si="3"/>
         <v>20800</v>
       </c>
-      <c r="H18" s="15">
+      <c r="H18" s="14">
         <v>5000</v>
       </c>
       <c r="I18" s="4"/>
@@ -3144,7 +3143,7 @@
       <c r="D19" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="E19" s="14" t="s">
+      <c r="E19" s="13" t="s">
         <v>34</v>
       </c>
       <c r="F19" s="1">
@@ -3155,7 +3154,7 @@
         <f t="shared" si="3"/>
         <v>12480</v>
       </c>
-      <c r="H19" s="15">
+      <c r="H19" s="14">
         <v>0</v>
       </c>
       <c r="I19" s="4"/>
@@ -3180,10 +3179,10 @@
       <c r="X19" s="4"/>
       <c r="Y19" s="4"/>
       <c r="Z19" s="4"/>
-      <c r="AA19" s="20">
-        <v>2080</v>
-      </c>
-      <c r="AB19" s="20">
+      <c r="AA19" s="19">
+        <v>2080</v>
+      </c>
+      <c r="AB19" s="19">
         <v>2080</v>
       </c>
       <c r="AC19" s="4"/>
@@ -3209,7 +3208,7 @@
       <c r="D20" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="E20" s="14" t="s">
+      <c r="E20" s="13" t="s">
         <v>35</v>
       </c>
       <c r="F20" s="1">
@@ -3220,7 +3219,7 @@
         <f t="shared" si="3"/>
         <v>7280</v>
       </c>
-      <c r="H20" s="15">
+      <c r="H20" s="14">
         <v>0</v>
       </c>
       <c r="I20" s="4">
@@ -3272,7 +3271,7 @@
       <c r="D21" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="E21" s="14" t="s">
+      <c r="E21" s="13" t="s">
         <v>36</v>
       </c>
       <c r="F21" s="1">
@@ -3283,7 +3282,7 @@
         <f t="shared" si="3"/>
         <v>20800</v>
       </c>
-      <c r="H21" s="15">
+      <c r="H21" s="14">
         <v>5000</v>
       </c>
       <c r="I21" s="4"/>
@@ -3333,7 +3332,7 @@
       <c r="D22" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="E22" s="14" t="s">
+      <c r="E22" s="13" t="s">
         <v>37</v>
       </c>
       <c r="F22" s="1">
@@ -3344,7 +3343,7 @@
         <f t="shared" si="3"/>
         <v>8320</v>
       </c>
-      <c r="H22" s="15">
+      <c r="H22" s="14">
         <v>0</v>
       </c>
       <c r="I22" s="4">
@@ -3402,7 +3401,7 @@
       <c r="D23" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="E23" s="14" t="s">
+      <c r="E23" s="13" t="s">
         <v>38</v>
       </c>
       <c r="F23" s="1">
@@ -3413,7 +3412,7 @@
         <f t="shared" si="3"/>
         <v>15600</v>
       </c>
-      <c r="H23" s="15">
+      <c r="H23" s="14">
         <v>0</v>
       </c>
       <c r="I23" s="4"/>
@@ -3465,18 +3464,18 @@
       <c r="D24" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="E24" s="14" t="s">
+      <c r="E24" s="13" t="s">
         <v>39</v>
       </c>
       <c r="F24" s="1">
         <f t="shared" si="2"/>
-        <v>30000</v>
+        <v>35000</v>
       </c>
       <c r="G24" s="1">
         <f t="shared" si="3"/>
-        <v>26000</v>
-      </c>
-      <c r="H24" s="15">
+        <v>31200</v>
+      </c>
+      <c r="H24" s="14">
         <v>5000</v>
       </c>
       <c r="I24" s="4"/>
@@ -3515,7 +3514,9 @@
       <c r="AF24" s="4"/>
       <c r="AG24" s="4"/>
       <c r="AH24" s="4"/>
-      <c r="AI24" s="4"/>
+      <c r="AI24" s="4">
+        <v>5200</v>
+      </c>
       <c r="AJ24" s="4"/>
       <c r="AK24" s="4"/>
       <c r="AL24" s="4"/>
@@ -3528,7 +3529,7 @@
       <c r="D25" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="E25" s="14" t="s">
+      <c r="E25" s="13" t="s">
         <v>40</v>
       </c>
       <c r="F25" s="1">
@@ -3539,7 +3540,7 @@
         <f t="shared" si="3"/>
         <v>24960</v>
       </c>
-      <c r="H25" s="15">
+      <c r="H25" s="14">
         <v>3000</v>
       </c>
       <c r="I25" s="4"/>
@@ -3597,18 +3598,18 @@
       <c r="D26" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="E26" s="14" t="s">
+      <c r="E26" s="13" t="s">
         <v>41</v>
       </c>
       <c r="F26" s="1">
         <f t="shared" si="2"/>
-        <v>10500</v>
+        <v>12500</v>
       </c>
       <c r="G26" s="1">
         <f t="shared" si="3"/>
-        <v>10400</v>
-      </c>
-      <c r="H26" s="15">
+        <v>12480</v>
+      </c>
+      <c r="H26" s="14">
         <v>500</v>
       </c>
       <c r="I26" s="4">
@@ -3647,7 +3648,9 @@
       <c r="AF26" s="4"/>
       <c r="AG26" s="4"/>
       <c r="AH26" s="4"/>
-      <c r="AI26" s="4"/>
+      <c r="AI26" s="4">
+        <v>2080</v>
+      </c>
       <c r="AJ26" s="4"/>
       <c r="AK26" s="4"/>
       <c r="AL26" s="4"/>
@@ -3660,7 +3663,7 @@
       <c r="D27" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="E27" s="14" t="s">
+      <c r="E27" s="13" t="s">
         <v>42</v>
       </c>
       <c r="F27" s="1">
@@ -3671,7 +3674,7 @@
         <f t="shared" si="3"/>
         <v>6240</v>
       </c>
-      <c r="H27" s="15">
+      <c r="H27" s="14">
         <v>0</v>
       </c>
       <c r="I27" s="4">
@@ -3719,7 +3722,7 @@
       <c r="D28" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="E28" s="14" t="s">
+      <c r="E28" s="13" t="s">
         <v>43</v>
       </c>
       <c r="F28" s="1">
@@ -3730,7 +3733,7 @@
         <f t="shared" si="3"/>
         <v>6240</v>
       </c>
-      <c r="H28" s="15">
+      <c r="H28" s="14">
         <v>0</v>
       </c>
       <c r="I28" s="4"/>
@@ -3778,7 +3781,7 @@
       <c r="D29" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="E29" s="14" t="s">
+      <c r="E29" s="13" t="s">
         <v>44</v>
       </c>
       <c r="F29" s="1">
@@ -3789,7 +3792,7 @@
         <f t="shared" si="3"/>
         <v>21840</v>
       </c>
-      <c r="H29" s="15">
+      <c r="H29" s="14">
         <v>0</v>
       </c>
       <c r="I29" s="4"/>
@@ -3823,7 +3826,7 @@
       <c r="AE29" s="4"/>
       <c r="AF29" s="4"/>
       <c r="AG29" s="4"/>
-      <c r="AH29" s="20">
+      <c r="AH29" s="19">
         <v>6240</v>
       </c>
       <c r="AI29" s="4"/>
@@ -3839,7 +3842,7 @@
       <c r="D30" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="E30" s="14" t="s">
+      <c r="E30" s="13" t="s">
         <v>45</v>
       </c>
       <c r="F30" s="1">
@@ -3850,7 +3853,7 @@
         <f t="shared" si="3"/>
         <v>46800</v>
       </c>
-      <c r="H30" s="15">
+      <c r="H30" s="14">
         <v>5000</v>
       </c>
       <c r="I30" s="4">
@@ -3910,7 +3913,7 @@
       <c r="D31" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="E31" s="14" t="s">
+      <c r="E31" s="13" t="s">
         <v>46</v>
       </c>
       <c r="F31" s="1">
@@ -3921,7 +3924,7 @@
         <f t="shared" si="3"/>
         <v>8320</v>
       </c>
-      <c r="H31" s="15">
+      <c r="H31" s="14">
         <v>0</v>
       </c>
       <c r="I31" s="4"/>
@@ -3971,7 +3974,7 @@
       <c r="D32" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="E32" s="14" t="s">
+      <c r="E32" s="13" t="s">
         <v>48</v>
       </c>
       <c r="F32" s="1">
@@ -3982,7 +3985,7 @@
         <f t="shared" si="3"/>
         <v>6240</v>
       </c>
-      <c r="H32" s="15">
+      <c r="H32" s="14">
         <v>1000</v>
       </c>
       <c r="I32" s="4"/>
@@ -4027,7 +4030,7 @@
       <c r="D33" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="E33" s="14" t="s">
+      <c r="E33" s="13" t="s">
         <v>49</v>
       </c>
       <c r="F33" s="1">
@@ -4038,7 +4041,7 @@
         <f t="shared" si="3"/>
         <v>5200</v>
       </c>
-      <c r="H33" s="15">
+      <c r="H33" s="14">
         <v>0</v>
       </c>
       <c r="I33" s="4"/>
@@ -4090,7 +4093,7 @@
       <c r="D34" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="E34" s="14" t="s">
+      <c r="E34" s="13" t="s">
         <v>50</v>
       </c>
       <c r="F34" s="1">
@@ -4101,7 +4104,7 @@
         <f t="shared" si="3"/>
         <v>8320</v>
       </c>
-      <c r="H34" s="15">
+      <c r="H34" s="14">
         <v>1000</v>
       </c>
       <c r="I34" s="4"/>
@@ -4151,7 +4154,7 @@
       <c r="D35" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="E35" s="14" t="s">
+      <c r="E35" s="13" t="s">
         <v>51</v>
       </c>
       <c r="F35" s="1">
@@ -4162,7 +4165,7 @@
         <f t="shared" si="3"/>
         <v>28080</v>
       </c>
-      <c r="H35" s="15">
+      <c r="H35" s="14">
         <v>0</v>
       </c>
       <c r="I35" s="4"/>
@@ -4222,7 +4225,7 @@
       <c r="D36" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="E36" s="14" t="s">
+      <c r="E36" s="13" t="s">
         <v>52</v>
       </c>
       <c r="F36" s="1">
@@ -4233,7 +4236,7 @@
         <f t="shared" ref="G36:G73" si="5">SUM(I36:AM36)</f>
         <v>3120</v>
       </c>
-      <c r="H36" s="15">
+      <c r="H36" s="14">
         <v>0</v>
       </c>
       <c r="I36" s="4"/>
@@ -4281,7 +4284,7 @@
       <c r="D37" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="E37" s="14" t="s">
+      <c r="E37" s="13" t="s">
         <v>53</v>
       </c>
       <c r="F37" s="1">
@@ -4292,14 +4295,14 @@
         <f t="shared" si="5"/>
         <v>18720</v>
       </c>
-      <c r="H37" s="15">
+      <c r="H37" s="14">
         <v>3000</v>
       </c>
       <c r="I37" s="4"/>
       <c r="J37" s="4"/>
       <c r="K37" s="4"/>
       <c r="L37" s="4"/>
-      <c r="M37" s="20">
+      <c r="M37" s="19">
         <v>3120</v>
       </c>
       <c r="N37" s="4"/>
@@ -4349,7 +4352,7 @@
       <c r="D38" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="E38" s="14" t="s">
+      <c r="E38" s="13" t="s">
         <v>54</v>
       </c>
       <c r="F38" s="1">
@@ -4360,7 +4363,7 @@
         <f t="shared" si="5"/>
         <v>4160</v>
       </c>
-      <c r="H38" s="15">
+      <c r="H38" s="14">
         <v>0</v>
       </c>
       <c r="I38" s="4"/>
@@ -4376,7 +4379,7 @@
       <c r="S38" s="4"/>
       <c r="T38" s="4"/>
       <c r="U38" s="4"/>
-      <c r="V38" s="20">
+      <c r="V38" s="19">
         <v>2080</v>
       </c>
       <c r="W38" s="4"/>
@@ -4387,7 +4390,7 @@
       <c r="AB38" s="4"/>
       <c r="AC38" s="4"/>
       <c r="AD38" s="4"/>
-      <c r="AE38" s="20">
+      <c r="AE38" s="19">
         <v>2080</v>
       </c>
       <c r="AF38" s="4"/>
@@ -4406,18 +4409,18 @@
       <c r="D39" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="E39" s="14" t="s">
+      <c r="E39" s="13" t="s">
         <v>55</v>
       </c>
       <c r="F39" s="1">
         <f t="shared" si="4"/>
-        <v>14000</v>
+        <v>16000</v>
       </c>
       <c r="G39" s="1">
         <f t="shared" si="5"/>
-        <v>14560</v>
-      </c>
-      <c r="H39" s="15">
+        <v>16640</v>
+      </c>
+      <c r="H39" s="14">
         <v>0</v>
       </c>
       <c r="I39" s="4"/>
@@ -4460,7 +4463,9 @@
       <c r="AF39" s="4"/>
       <c r="AG39" s="4"/>
       <c r="AH39" s="4"/>
-      <c r="AI39" s="4"/>
+      <c r="AI39" s="4">
+        <v>2080</v>
+      </c>
       <c r="AJ39" s="4"/>
       <c r="AK39" s="4"/>
       <c r="AL39" s="4"/>
@@ -4473,7 +4478,7 @@
       <c r="D40" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="E40" s="14" t="s">
+      <c r="E40" s="13" t="s">
         <v>56</v>
       </c>
       <c r="F40" s="1">
@@ -4484,7 +4489,7 @@
         <f>SUM(J40:AM40)</f>
         <v>8320</v>
       </c>
-      <c r="H40" s="15">
+      <c r="H40" s="14">
         <v>0</v>
       </c>
       <c r="J40" s="4">
@@ -4533,7 +4538,7 @@
       <c r="D41" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="E41" s="14" t="s">
+      <c r="E41" s="13" t="s">
         <v>57</v>
       </c>
       <c r="F41" s="1">
@@ -4544,7 +4549,7 @@
         <f t="shared" si="5"/>
         <v>31200</v>
       </c>
-      <c r="H41" s="15">
+      <c r="H41" s="14">
         <v>3000</v>
       </c>
       <c r="I41" s="4">
@@ -4606,7 +4611,7 @@
       <c r="D42" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="E42" s="14" t="s">
+      <c r="E42" s="13" t="s">
         <v>58</v>
       </c>
       <c r="F42" s="1">
@@ -4617,7 +4622,7 @@
         <f t="shared" si="5"/>
         <v>4160</v>
       </c>
-      <c r="H42" s="15">
+      <c r="H42" s="14">
         <v>0</v>
       </c>
       <c r="I42" s="4">
@@ -4663,7 +4668,7 @@
       <c r="D43" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="E43" s="14" t="s">
+      <c r="E43" s="13" t="s">
         <v>59</v>
       </c>
       <c r="F43" s="1">
@@ -4674,7 +4679,7 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="H43" s="15">
+      <c r="H43" s="14">
         <v>0</v>
       </c>
       <c r="I43" s="4"/>
@@ -4716,7 +4721,7 @@
       <c r="D44" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="E44" s="14" t="s">
+      <c r="E44" s="13" t="s">
         <v>60</v>
       </c>
       <c r="F44" s="1">
@@ -4727,7 +4732,7 @@
         <f t="shared" si="5"/>
         <v>21840</v>
       </c>
-      <c r="H44" s="15">
+      <c r="H44" s="14">
         <v>3000</v>
       </c>
       <c r="I44" s="4"/>
@@ -4783,18 +4788,18 @@
       <c r="D45" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="E45" s="14" t="s">
+      <c r="E45" s="13" t="s">
         <v>62</v>
       </c>
       <c r="F45" s="1">
         <f t="shared" si="4"/>
-        <v>21000</v>
+        <v>24000</v>
       </c>
       <c r="G45" s="1">
         <f t="shared" si="5"/>
-        <v>18720</v>
-      </c>
-      <c r="H45" s="15">
+        <v>21840</v>
+      </c>
+      <c r="H45" s="14">
         <v>3000</v>
       </c>
       <c r="I45" s="4"/>
@@ -4835,7 +4840,9 @@
       </c>
       <c r="AG45" s="4"/>
       <c r="AH45" s="4"/>
-      <c r="AI45" s="4"/>
+      <c r="AI45" s="4">
+        <v>3120</v>
+      </c>
       <c r="AJ45" s="4"/>
       <c r="AK45" s="4"/>
       <c r="AL45" s="4"/>
@@ -4848,7 +4855,7 @@
       <c r="D46" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="E46" s="14" t="s">
+      <c r="E46" s="13" t="s">
         <v>63</v>
       </c>
       <c r="F46" s="1">
@@ -4859,7 +4866,7 @@
         <f t="shared" si="5"/>
         <v>15600</v>
       </c>
-      <c r="H46" s="15">
+      <c r="H46" s="14">
         <v>0</v>
       </c>
       <c r="I46" s="4"/>
@@ -4911,7 +4918,7 @@
       <c r="D47" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="E47" s="14" t="s">
+      <c r="E47" s="13" t="s">
         <v>64</v>
       </c>
       <c r="F47" s="1">
@@ -4922,7 +4929,7 @@
         <f t="shared" si="5"/>
         <v>4160</v>
       </c>
-      <c r="H47" s="15">
+      <c r="H47" s="14">
         <v>0</v>
       </c>
       <c r="I47" s="4"/>
@@ -4968,7 +4975,7 @@
       <c r="D48" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="E48" s="14" t="s">
+      <c r="E48" s="13" t="s">
         <v>65</v>
       </c>
       <c r="F48" s="1">
@@ -4979,7 +4986,7 @@
         <f t="shared" si="5"/>
         <v>21840</v>
       </c>
-      <c r="H48" s="15">
+      <c r="H48" s="14">
         <v>3000</v>
       </c>
       <c r="I48" s="4">
@@ -5035,18 +5042,18 @@
       <c r="D49" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="E49" s="14" t="s">
+      <c r="E49" s="13" t="s">
         <v>66</v>
       </c>
       <c r="F49" s="1">
         <f t="shared" si="4"/>
-        <v>24000</v>
+        <v>27000</v>
       </c>
       <c r="G49" s="1">
         <f t="shared" si="5"/>
-        <v>21840</v>
-      </c>
-      <c r="H49" s="15">
+        <v>24960</v>
+      </c>
+      <c r="H49" s="14">
         <v>3000</v>
       </c>
       <c r="I49" s="4"/>
@@ -5089,7 +5096,9 @@
       </c>
       <c r="AG49" s="4"/>
       <c r="AH49" s="4"/>
-      <c r="AI49" s="4"/>
+      <c r="AI49" s="4">
+        <v>3120</v>
+      </c>
       <c r="AJ49" s="4"/>
       <c r="AK49" s="4"/>
       <c r="AL49" s="4"/>
@@ -5102,7 +5111,7 @@
       <c r="D50" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="E50" s="14" t="s">
+      <c r="E50" s="13" t="s">
         <v>67</v>
       </c>
       <c r="F50" s="1">
@@ -5113,7 +5122,7 @@
         <f t="shared" si="5"/>
         <v>6240</v>
       </c>
-      <c r="H50" s="15">
+      <c r="H50" s="14">
         <v>2000</v>
       </c>
       <c r="I50" s="4"/>
@@ -5161,7 +5170,7 @@
       <c r="D51" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="E51" s="14" t="s">
+      <c r="E51" s="13" t="s">
         <v>68</v>
       </c>
       <c r="F51" s="1">
@@ -5172,7 +5181,7 @@
         <f t="shared" si="5"/>
         <v>2080</v>
       </c>
-      <c r="H51" s="15">
+      <c r="H51" s="14">
         <v>0</v>
       </c>
       <c r="I51" s="4"/>
@@ -5216,18 +5225,18 @@
       <c r="D52" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="E52" s="14" t="s">
+      <c r="E52" s="13" t="s">
         <v>69</v>
       </c>
       <c r="F52" s="1">
         <f t="shared" si="4"/>
-        <v>19000</v>
+        <v>20000</v>
       </c>
       <c r="G52" s="1">
         <f t="shared" si="5"/>
-        <v>16640</v>
-      </c>
-      <c r="H52" s="15">
+        <v>17680</v>
+      </c>
+      <c r="H52" s="14">
         <v>3000</v>
       </c>
       <c r="I52" s="4">
@@ -5284,7 +5293,9 @@
       </c>
       <c r="AG52" s="4"/>
       <c r="AH52" s="4"/>
-      <c r="AI52" s="4"/>
+      <c r="AI52" s="4">
+        <v>1040</v>
+      </c>
       <c r="AJ52" s="4"/>
       <c r="AK52" s="4"/>
       <c r="AL52" s="4"/>
@@ -5294,11 +5305,11 @@
       <c r="A53" s="3">
         <v>51</v>
       </c>
-      <c r="B53" s="16"/>
+      <c r="B53" s="15"/>
       <c r="D53" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="E53" s="17" t="s">
+      <c r="E53" s="16" t="s">
         <v>70</v>
       </c>
       <c r="F53" s="1">
@@ -5309,7 +5320,7 @@
         <f t="shared" si="5"/>
         <v>16640</v>
       </c>
-      <c r="H53" s="15">
+      <c r="H53" s="14">
         <v>1000</v>
       </c>
       <c r="I53" s="4"/>
@@ -5379,18 +5390,18 @@
       <c r="D54" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="E54" s="14" t="s">
+      <c r="E54" s="13" t="s">
         <v>72</v>
       </c>
       <c r="F54" s="1">
         <f t="shared" si="4"/>
-        <v>10000</v>
+        <v>12000</v>
       </c>
       <c r="G54" s="1">
         <f t="shared" si="5"/>
-        <v>8320</v>
-      </c>
-      <c r="H54" s="15">
+        <v>10400</v>
+      </c>
+      <c r="H54" s="14">
         <v>2000</v>
       </c>
       <c r="I54" s="4"/>
@@ -5427,7 +5438,9 @@
       </c>
       <c r="AG54" s="4"/>
       <c r="AH54" s="4"/>
-      <c r="AI54" s="4"/>
+      <c r="AI54" s="4">
+        <v>2080</v>
+      </c>
       <c r="AJ54" s="4"/>
       <c r="AK54" s="4"/>
       <c r="AL54" s="4"/>
@@ -5440,7 +5453,7 @@
       <c r="D55" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="E55" s="14" t="s">
+      <c r="E55" s="13" t="s">
         <v>73</v>
       </c>
       <c r="F55" s="1">
@@ -5451,7 +5464,7 @@
         <f t="shared" si="5"/>
         <v>36400</v>
       </c>
-      <c r="H55" s="15">
+      <c r="H55" s="14">
         <v>0</v>
       </c>
       <c r="I55" s="4"/>
@@ -5507,7 +5520,7 @@
       <c r="D56" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="E56" s="14" t="s">
+      <c r="E56" s="13" t="s">
         <v>74</v>
       </c>
       <c r="F56" s="1">
@@ -5518,7 +5531,7 @@
         <f t="shared" si="5"/>
         <v>8320</v>
       </c>
-      <c r="H56" s="15">
+      <c r="H56" s="14">
         <v>0</v>
       </c>
       <c r="I56" s="4"/>
@@ -5565,11 +5578,11 @@
       <c r="A57" s="3">
         <v>55</v>
       </c>
-      <c r="B57" s="16"/>
+      <c r="B57" s="15"/>
       <c r="D57" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="E57" s="17" t="s">
+      <c r="E57" s="16" t="s">
         <v>76</v>
       </c>
       <c r="F57" s="1">
@@ -5580,7 +5593,7 @@
         <f t="shared" si="5"/>
         <v>31200</v>
       </c>
-      <c r="H57" s="15">
+      <c r="H57" s="14">
         <v>5000</v>
       </c>
       <c r="I57" s="4"/>
@@ -5631,13 +5644,13 @@
       <c r="A58" s="3">
         <v>56</v>
       </c>
-      <c r="C58" s="18" t="s">
+      <c r="C58" s="17" t="s">
         <v>77</v>
       </c>
       <c r="D58" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="E58" s="14" t="s">
+      <c r="E58" s="13" t="s">
         <v>78</v>
       </c>
       <c r="F58" s="1">
@@ -5648,13 +5661,13 @@
         <f t="shared" si="5"/>
         <v>10400</v>
       </c>
-      <c r="H58" s="15">
+      <c r="H58" s="14">
         <v>0</v>
       </c>
       <c r="I58" s="4"/>
       <c r="J58" s="4"/>
       <c r="K58" s="4"/>
-      <c r="L58" s="20">
+      <c r="L58" s="19">
         <v>5200</v>
       </c>
       <c r="M58" s="4"/>
@@ -5691,11 +5704,11 @@
       <c r="A59" s="3">
         <v>57</v>
       </c>
-      <c r="B59" s="16"/>
+      <c r="B59" s="15"/>
       <c r="D59" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="E59" s="17" t="s">
+      <c r="E59" s="16" t="s">
         <v>80</v>
       </c>
       <c r="F59" s="1">
@@ -5706,7 +5719,7 @@
         <f t="shared" si="5"/>
         <v>20800</v>
       </c>
-      <c r="H59" s="15">
+      <c r="H59" s="14">
         <v>1000</v>
       </c>
       <c r="I59" s="4">
@@ -5765,11 +5778,11 @@
       <c r="A60" s="3">
         <v>58</v>
       </c>
-      <c r="B60" s="16"/>
+      <c r="B60" s="15"/>
       <c r="D60" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="E60" s="17" t="s">
+      <c r="E60" s="16" t="s">
         <v>82</v>
       </c>
       <c r="F60" s="1">
@@ -5780,7 +5793,7 @@
         <f t="shared" si="5"/>
         <v>6240</v>
       </c>
-      <c r="H60" s="15">
+      <c r="H60" s="14">
         <v>2000</v>
       </c>
       <c r="I60" s="4"/>
@@ -5828,7 +5841,7 @@
       <c r="D61" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="E61" s="14" t="s">
+      <c r="E61" s="13" t="s">
         <v>84</v>
       </c>
       <c r="F61" s="1">
@@ -5839,7 +5852,7 @@
         <f t="shared" si="5"/>
         <v>14560</v>
       </c>
-      <c r="H61" s="15">
+      <c r="H61" s="14">
         <v>0</v>
       </c>
       <c r="I61" s="4"/>
@@ -5873,7 +5886,7 @@
       <c r="AB61" s="4"/>
       <c r="AC61" s="4"/>
       <c r="AD61" s="4"/>
-      <c r="AE61" s="20">
+      <c r="AE61" s="19">
         <v>2080</v>
       </c>
       <c r="AF61" s="4"/>
@@ -5894,7 +5907,7 @@
       <c r="D62" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="E62" s="14" t="s">
+      <c r="E62" s="13" t="s">
         <v>85</v>
       </c>
       <c r="F62" s="1">
@@ -5905,7 +5918,7 @@
         <f t="shared" si="5"/>
         <v>10400</v>
       </c>
-      <c r="H62" s="15">
+      <c r="H62" s="14">
         <v>0</v>
       </c>
       <c r="I62" s="4"/>
@@ -5957,7 +5970,7 @@
       <c r="D63" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="E63" s="14" t="s">
+      <c r="E63" s="13" t="s">
         <v>86</v>
       </c>
       <c r="F63" s="1">
@@ -5968,7 +5981,7 @@
         <f t="shared" si="5"/>
         <v>6240</v>
       </c>
-      <c r="H63" s="15">
+      <c r="H63" s="14">
         <v>0</v>
       </c>
       <c r="I63" s="4"/>
@@ -6016,7 +6029,7 @@
       <c r="D64" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="E64" s="14" t="s">
+      <c r="E64" s="13" t="s">
         <v>87</v>
       </c>
       <c r="F64" s="1">
@@ -6027,7 +6040,7 @@
         <f t="shared" si="5"/>
         <v>3120</v>
       </c>
-      <c r="H64" s="15">
+      <c r="H64" s="14">
         <v>0</v>
       </c>
       <c r="I64" s="4"/>
@@ -6075,7 +6088,7 @@
       <c r="D65" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="E65" s="14" t="s">
+      <c r="E65" s="13" t="s">
         <v>88</v>
       </c>
       <c r="F65" s="1">
@@ -6086,7 +6099,7 @@
         <f t="shared" si="5"/>
         <v>52000</v>
       </c>
-      <c r="H65" s="15">
+      <c r="H65" s="14">
         <v>0</v>
       </c>
       <c r="I65" s="4">
@@ -6148,7 +6161,7 @@
       <c r="D66" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="E66" s="14" t="s">
+      <c r="E66" s="13" t="s">
         <v>89</v>
       </c>
       <c r="F66" s="1">
@@ -6159,7 +6172,7 @@
         <f t="shared" si="5"/>
         <v>24960</v>
       </c>
-      <c r="H66" s="15">
+      <c r="H66" s="14">
         <v>3000</v>
       </c>
       <c r="I66" s="4"/>
@@ -6213,11 +6226,11 @@
       <c r="A67" s="3">
         <v>65</v>
       </c>
-      <c r="B67" s="16"/>
+      <c r="B67" s="15"/>
       <c r="D67" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="E67" s="17" t="s">
+      <c r="E67" s="16" t="s">
         <v>90</v>
       </c>
       <c r="F67" s="1">
@@ -6228,7 +6241,7 @@
         <f t="shared" si="5"/>
         <v>14560</v>
       </c>
-      <c r="H67" s="15">
+      <c r="H67" s="14">
         <v>2000</v>
       </c>
       <c r="I67" s="4">
@@ -6281,11 +6294,11 @@
       <c r="A68" s="3">
         <v>66</v>
       </c>
-      <c r="B68" s="16"/>
+      <c r="B68" s="15"/>
       <c r="D68" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="E68" s="17" t="s">
+      <c r="E68" s="16" t="s">
         <v>91</v>
       </c>
       <c r="F68" s="1">
@@ -6296,7 +6309,7 @@
         <f t="shared" si="5"/>
         <v>2080</v>
       </c>
-      <c r="H68" s="15">
+      <c r="H68" s="14">
         <v>500</v>
       </c>
       <c r="I68" s="4"/>
@@ -6340,18 +6353,18 @@
       <c r="D69" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="E69" s="14" t="s">
+      <c r="E69" s="13" t="s">
         <v>93</v>
       </c>
       <c r="F69" s="1">
         <f t="shared" si="6"/>
-        <v>15500</v>
+        <v>16500</v>
       </c>
       <c r="G69" s="1">
         <f t="shared" si="5"/>
-        <v>14560</v>
-      </c>
-      <c r="H69" s="15">
+        <v>15600</v>
+      </c>
+      <c r="H69" s="14">
         <v>1500</v>
       </c>
       <c r="I69" s="4">
@@ -6398,7 +6411,9 @@
       </c>
       <c r="AG69" s="4"/>
       <c r="AH69" s="4"/>
-      <c r="AI69" s="4"/>
+      <c r="AI69" s="4">
+        <v>1040</v>
+      </c>
       <c r="AJ69" s="4"/>
       <c r="AK69" s="4"/>
       <c r="AL69" s="4"/>
@@ -6411,7 +6426,7 @@
       <c r="D70" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="E70" s="14" t="s">
+      <c r="E70" s="13" t="s">
         <v>94</v>
       </c>
       <c r="F70" s="1">
@@ -6422,7 +6437,7 @@
         <f t="shared" si="5"/>
         <v>28080</v>
       </c>
-      <c r="H70" s="15">
+      <c r="H70" s="14">
         <v>0</v>
       </c>
       <c r="I70" s="4"/>
@@ -6482,7 +6497,7 @@
       <c r="D71" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="E71" s="14" t="s">
+      <c r="E71" s="13" t="s">
         <v>95</v>
       </c>
       <c r="F71" s="1">
@@ -6493,7 +6508,7 @@
         <f t="shared" si="5"/>
         <v>22880</v>
       </c>
-      <c r="H71" s="15">
+      <c r="H71" s="14">
         <v>2000</v>
       </c>
       <c r="I71" s="4"/>
@@ -6554,8 +6569,8 @@
       <c r="A72" s="3">
         <v>70</v>
       </c>
-      <c r="B72" s="16"/>
-      <c r="E72" s="17" t="s">
+      <c r="B72" s="15"/>
+      <c r="E72" s="16" t="s">
         <v>96</v>
       </c>
       <c r="F72" s="1">
@@ -6566,40 +6581,40 @@
         <f t="shared" si="5"/>
         <v>20800</v>
       </c>
-      <c r="H72" s="15">
+      <c r="H72" s="14">
         <v>27000</v>
       </c>
-      <c r="I72" s="23"/>
-      <c r="J72" s="23"/>
-      <c r="K72" s="23"/>
-      <c r="L72" s="23">
-        <v>2080</v>
-      </c>
-      <c r="M72" s="24">
+      <c r="I72" s="22"/>
+      <c r="J72" s="22"/>
+      <c r="K72" s="22"/>
+      <c r="L72" s="22">
+        <v>2080</v>
+      </c>
+      <c r="M72" s="23">
         <v>4160</v>
       </c>
-      <c r="N72" s="23">
-        <v>2080</v>
-      </c>
-      <c r="O72" s="23"/>
-      <c r="P72" s="23"/>
-      <c r="Q72" s="23">
-        <v>2080</v>
-      </c>
-      <c r="R72" s="23"/>
-      <c r="S72" s="23">
-        <v>2080</v>
-      </c>
-      <c r="T72" s="23">
+      <c r="N72" s="22">
+        <v>2080</v>
+      </c>
+      <c r="O72" s="22"/>
+      <c r="P72" s="22"/>
+      <c r="Q72" s="22">
+        <v>2080</v>
+      </c>
+      <c r="R72" s="22"/>
+      <c r="S72" s="22">
+        <v>2080</v>
+      </c>
+      <c r="T72" s="22">
         <v>2080</v>
       </c>
       <c r="U72" s="4">
         <v>2080</v>
       </c>
-      <c r="V72" s="25"/>
-      <c r="W72" s="25"/>
-      <c r="X72" s="25"/>
-      <c r="Y72" s="25"/>
+      <c r="V72" s="24"/>
+      <c r="W72" s="24"/>
+      <c r="X72" s="24"/>
+      <c r="Y72" s="24"/>
       <c r="Z72" s="4"/>
       <c r="AA72" s="4"/>
       <c r="AB72" s="4">
@@ -6623,11 +6638,11 @@
       <c r="A73" s="3">
         <v>71</v>
       </c>
-      <c r="B73" s="16"/>
+      <c r="B73" s="15"/>
       <c r="D73" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="E73" s="17" t="s">
+      <c r="E73" s="16" t="s">
         <v>98</v>
       </c>
       <c r="F73" s="1">
@@ -6638,7 +6653,7 @@
         <f t="shared" si="5"/>
         <v>6240</v>
       </c>
-      <c r="H73" s="15">
+      <c r="H73" s="14">
         <v>0</v>
       </c>
       <c r="I73" s="4"/>
@@ -6647,7 +6662,7 @@
       <c r="L73" s="4"/>
       <c r="M73" s="4"/>
       <c r="N73" s="4"/>
-      <c r="O73" s="20">
+      <c r="O73" s="19">
         <v>3120</v>
       </c>
       <c r="P73" s="4"/>
@@ -6683,8 +6698,8 @@
       <c r="A74" s="3">
         <v>72</v>
       </c>
-      <c r="B74" s="16"/>
-      <c r="E74" s="17" t="s">
+      <c r="B74" s="15"/>
+      <c r="E74" s="16" t="s">
         <v>99</v>
       </c>
       <c r="F74" s="1">
@@ -6695,7 +6710,7 @@
         <f t="shared" ref="G69:G95" si="7">SUM(I74:AM74)</f>
         <v>0</v>
       </c>
-      <c r="H74" s="15">
+      <c r="H74" s="14">
         <v>0</v>
       </c>
       <c r="I74" s="4"/>
@@ -6734,11 +6749,11 @@
       <c r="A75" s="3">
         <v>73</v>
       </c>
-      <c r="B75" s="16"/>
+      <c r="B75" s="15"/>
       <c r="D75" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="E75" s="17" t="s">
+      <c r="E75" s="16" t="s">
         <v>101</v>
       </c>
       <c r="F75" s="1">
@@ -6749,14 +6764,14 @@
         <f t="shared" si="7"/>
         <v>6240</v>
       </c>
-      <c r="H75" s="15">
+      <c r="H75" s="14">
         <v>0</v>
       </c>
       <c r="I75" s="4"/>
       <c r="J75" s="4"/>
       <c r="K75" s="4"/>
       <c r="L75" s="4"/>
-      <c r="M75" s="20">
+      <c r="M75" s="19">
         <v>1040</v>
       </c>
       <c r="N75" s="4">
@@ -6796,8 +6811,8 @@
       <c r="A76" s="3">
         <v>74</v>
       </c>
-      <c r="B76" s="16"/>
-      <c r="E76" s="17" t="s">
+      <c r="B76" s="15"/>
+      <c r="E76" s="16" t="s">
         <v>102</v>
       </c>
       <c r="F76" s="1">
@@ -6808,21 +6823,21 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="H76" s="15">
-        <v>0</v>
-      </c>
-      <c r="I76" s="25"/>
-      <c r="J76" s="25"/>
-      <c r="K76" s="25"/>
-      <c r="L76" s="25"/>
-      <c r="M76" s="25"/>
-      <c r="N76" s="25"/>
-      <c r="O76" s="25"/>
-      <c r="P76" s="25"/>
-      <c r="Q76" s="25"/>
-      <c r="R76" s="25"/>
-      <c r="S76" s="25"/>
-      <c r="T76" s="25"/>
+      <c r="H76" s="14">
+        <v>0</v>
+      </c>
+      <c r="I76" s="24"/>
+      <c r="J76" s="24"/>
+      <c r="K76" s="24"/>
+      <c r="L76" s="24"/>
+      <c r="M76" s="24"/>
+      <c r="N76" s="24"/>
+      <c r="O76" s="24"/>
+      <c r="P76" s="24"/>
+      <c r="Q76" s="24"/>
+      <c r="R76" s="24"/>
+      <c r="S76" s="24"/>
+      <c r="T76" s="24"/>
       <c r="U76" s="4"/>
       <c r="V76" s="4"/>
       <c r="W76" s="4"/>
@@ -6847,14 +6862,14 @@
       <c r="A77" s="3">
         <v>75</v>
       </c>
-      <c r="B77" s="16"/>
+      <c r="B77" s="15"/>
       <c r="C77" s="3">
         <v>683879115</v>
       </c>
       <c r="D77" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="E77" s="17" t="s">
+      <c r="E77" s="16" t="s">
         <v>104</v>
       </c>
       <c r="F77" s="1">
@@ -6865,7 +6880,7 @@
         <f t="shared" si="7"/>
         <v>6240</v>
       </c>
-      <c r="H77" s="15">
+      <c r="H77" s="14">
         <v>0</v>
       </c>
       <c r="I77" s="4"/>
@@ -6894,7 +6909,7 @@
       <c r="AB77" s="4"/>
       <c r="AC77" s="4"/>
       <c r="AD77" s="4"/>
-      <c r="AE77" s="20">
+      <c r="AE77" s="19">
         <v>2080</v>
       </c>
       <c r="AF77" s="4"/>
@@ -6910,11 +6925,11 @@
       <c r="A78" s="3">
         <v>76</v>
       </c>
-      <c r="B78" s="16"/>
+      <c r="B78" s="15"/>
       <c r="D78" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="E78" s="17" t="s">
+      <c r="E78" s="16" t="s">
         <v>105</v>
       </c>
       <c r="F78" s="1">
@@ -6925,7 +6940,7 @@
         <f t="shared" si="7"/>
         <v>4160</v>
       </c>
-      <c r="H78" s="15">
+      <c r="H78" s="14">
         <v>0</v>
       </c>
       <c r="I78" s="4"/>
@@ -6935,7 +6950,7 @@
       <c r="M78" s="4"/>
       <c r="N78" s="4"/>
       <c r="O78" s="4"/>
-      <c r="P78" s="20">
+      <c r="P78" s="19">
         <v>2080</v>
       </c>
       <c r="Q78" s="4"/>
@@ -6952,7 +6967,7 @@
       <c r="AB78" s="4"/>
       <c r="AC78" s="4"/>
       <c r="AD78" s="4"/>
-      <c r="AE78" s="20">
+      <c r="AE78" s="19">
         <v>2080</v>
       </c>
       <c r="AF78" s="4"/>
@@ -6968,8 +6983,8 @@
       <c r="A79" s="3">
         <v>77</v>
       </c>
-      <c r="B79" s="16"/>
-      <c r="E79" s="17" t="s">
+      <c r="B79" s="15"/>
+      <c r="E79" s="16" t="s">
         <v>106</v>
       </c>
       <c r="F79" s="1">
@@ -6980,7 +6995,7 @@
         <f t="shared" si="7"/>
         <v>4160</v>
       </c>
-      <c r="H79" s="15">
+      <c r="H79" s="14">
         <v>0</v>
       </c>
       <c r="I79" s="4"/>
@@ -7023,11 +7038,11 @@
       <c r="A80" s="3">
         <v>78</v>
       </c>
-      <c r="B80" s="16"/>
+      <c r="B80" s="15"/>
       <c r="D80" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="E80" s="17" t="s">
+      <c r="E80" s="16" t="s">
         <v>107</v>
       </c>
       <c r="F80" s="1">
@@ -7038,7 +7053,7 @@
         <f t="shared" si="7"/>
         <v>7280</v>
       </c>
-      <c r="H80" s="15">
+      <c r="H80" s="14">
         <v>0</v>
       </c>
       <c r="I80" s="4"/>
@@ -7053,7 +7068,7 @@
       <c r="R80" s="4"/>
       <c r="S80" s="4"/>
       <c r="T80" s="4"/>
-      <c r="U80" s="20">
+      <c r="U80" s="19">
         <v>2080</v>
       </c>
       <c r="V80" s="4"/>
@@ -7089,11 +7104,11 @@
       <c r="A81" s="3">
         <v>79</v>
       </c>
-      <c r="B81" s="16"/>
+      <c r="B81" s="15"/>
       <c r="D81" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="E81" s="17" t="s">
+      <c r="E81" s="16" t="s">
         <v>109</v>
       </c>
       <c r="F81" s="1">
@@ -7104,31 +7119,31 @@
         <f t="shared" si="7"/>
         <v>6240</v>
       </c>
-      <c r="H81" s="15">
-        <v>0</v>
-      </c>
-      <c r="I81" s="25"/>
-      <c r="J81" s="25"/>
-      <c r="K81" s="25"/>
-      <c r="L81" s="25"/>
-      <c r="M81" s="25"/>
-      <c r="N81" s="25"/>
-      <c r="O81" s="23">
-        <v>2080</v>
-      </c>
-      <c r="P81" s="25"/>
-      <c r="Q81" s="25"/>
-      <c r="R81" s="25"/>
-      <c r="S81" s="25"/>
-      <c r="T81" s="25"/>
-      <c r="U81" s="25"/>
-      <c r="V81" s="25"/>
-      <c r="W81" s="23">
-        <v>2080</v>
-      </c>
-      <c r="X81" s="25"/>
-      <c r="Y81" s="25"/>
-      <c r="Z81" s="25"/>
+      <c r="H81" s="14">
+        <v>0</v>
+      </c>
+      <c r="I81" s="24"/>
+      <c r="J81" s="24"/>
+      <c r="K81" s="24"/>
+      <c r="L81" s="24"/>
+      <c r="M81" s="24"/>
+      <c r="N81" s="24"/>
+      <c r="O81" s="22">
+        <v>2080</v>
+      </c>
+      <c r="P81" s="24"/>
+      <c r="Q81" s="24"/>
+      <c r="R81" s="24"/>
+      <c r="S81" s="24"/>
+      <c r="T81" s="24"/>
+      <c r="U81" s="24"/>
+      <c r="V81" s="24"/>
+      <c r="W81" s="22">
+        <v>2080</v>
+      </c>
+      <c r="X81" s="24"/>
+      <c r="Y81" s="24"/>
+      <c r="Z81" s="24"/>
       <c r="AA81" s="4"/>
       <c r="AB81" s="4">
         <v>2080</v>
@@ -7149,11 +7164,11 @@
       <c r="A82" s="3">
         <v>80</v>
       </c>
-      <c r="B82" s="16"/>
+      <c r="B82" s="15"/>
       <c r="D82" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="E82" s="17" t="s">
+      <c r="E82" s="16" t="s">
         <v>110</v>
       </c>
       <c r="F82" s="1">
@@ -7164,7 +7179,7 @@
         <f t="shared" si="7"/>
         <v>31200</v>
       </c>
-      <c r="H82" s="15">
+      <c r="H82" s="14">
         <v>0</v>
       </c>
       <c r="I82" s="4">
@@ -7215,8 +7230,8 @@
       <c r="A83" s="3">
         <v>81</v>
       </c>
-      <c r="B83" s="16"/>
-      <c r="E83" s="17" t="s">
+      <c r="B83" s="15"/>
+      <c r="E83" s="16" t="s">
         <v>111</v>
       </c>
       <c r="F83" s="1">
@@ -7227,7 +7242,7 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="H83" s="15">
+      <c r="H83" s="14">
         <v>0</v>
       </c>
       <c r="I83" s="4"/>
@@ -7266,8 +7281,8 @@
       <c r="A84" s="3">
         <v>82</v>
       </c>
-      <c r="B84" s="16"/>
-      <c r="E84" s="17" t="s">
+      <c r="B84" s="15"/>
+      <c r="E84" s="16" t="s">
         <v>112</v>
       </c>
       <c r="F84" s="1">
@@ -7278,20 +7293,20 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="H84" s="15">
-        <v>0</v>
-      </c>
-      <c r="I84" s="25"/>
-      <c r="J84" s="25"/>
-      <c r="K84" s="25"/>
-      <c r="L84" s="25"/>
-      <c r="M84" s="25"/>
-      <c r="N84" s="25"/>
-      <c r="O84" s="25"/>
-      <c r="P84" s="25"/>
-      <c r="Q84" s="25"/>
-      <c r="R84" s="25"/>
-      <c r="S84" s="25"/>
+      <c r="H84" s="14">
+        <v>0</v>
+      </c>
+      <c r="I84" s="24"/>
+      <c r="J84" s="24"/>
+      <c r="K84" s="24"/>
+      <c r="L84" s="24"/>
+      <c r="M84" s="24"/>
+      <c r="N84" s="24"/>
+      <c r="O84" s="24"/>
+      <c r="P84" s="24"/>
+      <c r="Q84" s="24"/>
+      <c r="R84" s="24"/>
+      <c r="S84" s="24"/>
       <c r="T84" s="4"/>
       <c r="U84" s="4"/>
       <c r="V84" s="4"/>
@@ -7317,11 +7332,11 @@
       <c r="A85" s="3">
         <v>83</v>
       </c>
-      <c r="B85" s="16"/>
+      <c r="B85" s="15"/>
       <c r="C85" s="3">
         <v>683909556</v>
       </c>
-      <c r="E85" s="17" t="s">
+      <c r="E85" s="16" t="s">
         <v>113</v>
       </c>
       <c r="F85" s="1">
@@ -7332,28 +7347,28 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="H85" s="15">
-        <v>0</v>
-      </c>
-      <c r="I85" s="25"/>
-      <c r="J85" s="25"/>
-      <c r="K85" s="25"/>
-      <c r="L85" s="25"/>
-      <c r="M85" s="25"/>
-      <c r="N85" s="25"/>
-      <c r="O85" s="25"/>
-      <c r="P85" s="25"/>
-      <c r="Q85" s="25"/>
-      <c r="R85" s="25"/>
-      <c r="S85" s="25"/>
-      <c r="T85" s="25"/>
-      <c r="U85" s="25"/>
-      <c r="V85" s="25"/>
-      <c r="W85" s="25"/>
-      <c r="X85" s="25"/>
-      <c r="Y85" s="25"/>
-      <c r="Z85" s="25"/>
-      <c r="AA85" s="25"/>
+      <c r="H85" s="14">
+        <v>0</v>
+      </c>
+      <c r="I85" s="24"/>
+      <c r="J85" s="24"/>
+      <c r="K85" s="24"/>
+      <c r="L85" s="24"/>
+      <c r="M85" s="24"/>
+      <c r="N85" s="24"/>
+      <c r="O85" s="24"/>
+      <c r="P85" s="24"/>
+      <c r="Q85" s="24"/>
+      <c r="R85" s="24"/>
+      <c r="S85" s="24"/>
+      <c r="T85" s="24"/>
+      <c r="U85" s="24"/>
+      <c r="V85" s="24"/>
+      <c r="W85" s="24"/>
+      <c r="X85" s="24"/>
+      <c r="Y85" s="24"/>
+      <c r="Z85" s="24"/>
+      <c r="AA85" s="24"/>
       <c r="AB85" s="4"/>
       <c r="AC85" s="4"/>
       <c r="AD85" s="4"/>
@@ -7371,8 +7386,8 @@
       <c r="A86" s="3">
         <v>84</v>
       </c>
-      <c r="B86" s="16"/>
-      <c r="E86" s="17" t="s">
+      <c r="B86" s="15"/>
+      <c r="E86" s="16" t="s">
         <v>114</v>
       </c>
       <c r="F86" s="1">
@@ -7383,25 +7398,25 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="H86" s="15">
-        <v>0</v>
-      </c>
-      <c r="I86" s="25"/>
-      <c r="J86" s="25"/>
-      <c r="K86" s="25"/>
-      <c r="L86" s="25"/>
-      <c r="M86" s="25"/>
-      <c r="N86" s="25"/>
-      <c r="O86" s="25"/>
-      <c r="P86" s="25"/>
-      <c r="Q86" s="25"/>
-      <c r="R86" s="25"/>
-      <c r="S86" s="25"/>
-      <c r="T86" s="25"/>
-      <c r="U86" s="25"/>
-      <c r="V86" s="25"/>
-      <c r="W86" s="25"/>
-      <c r="X86" s="25"/>
+      <c r="H86" s="14">
+        <v>0</v>
+      </c>
+      <c r="I86" s="24"/>
+      <c r="J86" s="24"/>
+      <c r="K86" s="24"/>
+      <c r="L86" s="24"/>
+      <c r="M86" s="24"/>
+      <c r="N86" s="24"/>
+      <c r="O86" s="24"/>
+      <c r="P86" s="24"/>
+      <c r="Q86" s="24"/>
+      <c r="R86" s="24"/>
+      <c r="S86" s="24"/>
+      <c r="T86" s="24"/>
+      <c r="U86" s="24"/>
+      <c r="V86" s="24"/>
+      <c r="W86" s="24"/>
+      <c r="X86" s="24"/>
       <c r="Y86" s="4"/>
       <c r="Z86" s="4"/>
       <c r="AA86" s="4"/>
@@ -7422,7 +7437,7 @@
       <c r="A87" s="3">
         <v>85</v>
       </c>
-      <c r="E87" s="14" t="s">
+      <c r="E87" s="13" t="s">
         <v>115</v>
       </c>
       <c r="F87" s="1">
@@ -7433,7 +7448,7 @@
         <f t="shared" si="7"/>
         <v>1040</v>
       </c>
-      <c r="H87" s="15">
+      <c r="H87" s="14">
         <v>0</v>
       </c>
       <c r="I87" s="4"/>
@@ -7474,7 +7489,7 @@
       <c r="A88" s="3">
         <v>86</v>
       </c>
-      <c r="E88" s="14" t="s">
+      <c r="E88" s="13" t="s">
         <v>116</v>
       </c>
       <c r="F88" s="1">
@@ -7485,7 +7500,7 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="H88" s="15">
+      <c r="H88" s="14">
         <v>0</v>
       </c>
       <c r="I88" s="4"/>
@@ -7524,7 +7539,7 @@
       <c r="A89" s="3">
         <v>87</v>
       </c>
-      <c r="E89" s="14" t="s">
+      <c r="E89" s="13" t="s">
         <v>117</v>
       </c>
       <c r="F89" s="1">
@@ -7535,7 +7550,7 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="H89" s="15">
+      <c r="H89" s="14">
         <v>0</v>
       </c>
       <c r="I89" s="4"/>
@@ -7577,7 +7592,7 @@
       <c r="D90" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="E90" s="14" t="s">
+      <c r="E90" s="13" t="s">
         <v>118</v>
       </c>
       <c r="F90" s="1">
@@ -7588,7 +7603,7 @@
         <f t="shared" si="7"/>
         <v>6240</v>
       </c>
-      <c r="H90" s="15">
+      <c r="H90" s="14">
         <v>0</v>
       </c>
       <c r="I90" s="4"/>
@@ -7634,7 +7649,7 @@
       <c r="D91" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="E91" s="14" t="s">
+      <c r="E91" s="13" t="s">
         <v>119</v>
       </c>
       <c r="F91" s="1">
@@ -7645,7 +7660,7 @@
         <f t="shared" si="7"/>
         <v>10400</v>
       </c>
-      <c r="H91" s="15">
+      <c r="H91" s="14">
         <v>0</v>
       </c>
       <c r="I91" s="4"/>
@@ -7691,7 +7706,7 @@
       <c r="C92" s="3">
         <v>683909558</v>
       </c>
-      <c r="E92" s="14" t="s">
+      <c r="E92" s="13" t="s">
         <v>120</v>
       </c>
       <c r="F92" s="1">
@@ -7702,7 +7717,7 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="H92" s="15">
+      <c r="H92" s="14">
         <v>0</v>
       </c>
       <c r="I92" s="4"/>
@@ -7741,7 +7756,7 @@
       <c r="A93" s="3">
         <v>91</v>
       </c>
-      <c r="E93" s="14" t="s">
+      <c r="E93" s="13" t="s">
         <v>121</v>
       </c>
       <c r="F93" s="1">
@@ -7752,7 +7767,7 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="H93" s="15">
+      <c r="H93" s="14">
         <v>0</v>
       </c>
       <c r="I93" s="4"/>
@@ -7791,7 +7806,7 @@
       <c r="A94" s="3">
         <v>92</v>
       </c>
-      <c r="E94" s="22" t="s">
+      <c r="E94" s="21" t="s">
         <v>122</v>
       </c>
       <c r="F94" s="1">
@@ -7802,7 +7817,7 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="H94" s="15">
+      <c r="H94" s="14">
         <v>0</v>
       </c>
       <c r="I94" s="4"/>
@@ -7865,13 +7880,13 @@
       <c r="J95" s="4"/>
       <c r="K95" s="4"/>
       <c r="L95" s="4"/>
-      <c r="M95" s="20">
+      <c r="M95" s="19">
         <v>2080</v>
       </c>
       <c r="N95" s="4"/>
       <c r="O95" s="4"/>
       <c r="P95" s="4"/>
-      <c r="Q95" s="20">
+      <c r="Q95" s="19">
         <v>2080</v>
       </c>
       <c r="R95" s="4"/>
@@ -7881,7 +7896,7 @@
       <c r="V95" s="4"/>
       <c r="W95" s="4"/>
       <c r="X95" s="4"/>
-      <c r="Y95" s="20">
+      <c r="Y95" s="19">
         <v>1040</v>
       </c>
       <c r="Z95" s="4"/>

</xml_diff>